<commit_message>
NDepend analysis & explanation
</commit_message>
<xml_diff>
--- a/data/codescene/codescene.xlsx
+++ b/data/codescene/codescene.xlsx
@@ -306,7 +306,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G6:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1022,7 +1022,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="G6:G10 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>